<commit_message>
Fixed celery tasks for working in docker. Updated docker files
</commit_message>
<xml_diff>
--- a/admin/Menu.xlsx
+++ b/admin/Menu.xlsx
@@ -1,38 +1,160 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Александр\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion1">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mjvwozj06heQVGmxYVZutM7iYW8Dw=="/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+  <si>
+    <t>Меню</t>
+  </si>
+  <si>
+    <t>Основное меню</t>
+  </si>
+  <si>
+    <t>Холодные закуски</t>
+  </si>
+  <si>
+    <t>К пиву</t>
+  </si>
+  <si>
+    <t>Сельдь Бисмарк</t>
+  </si>
+  <si>
+    <t>Традиционное немецкое блюдо из маринованной сельди</t>
+  </si>
+  <si>
+    <t>Мясная тарелка</t>
+  </si>
+  <si>
+    <t>Рыбная тарелка</t>
+  </si>
+  <si>
+    <t>Нарезка из креветок, кальмаров, раковых шеек, гребешков, лосося, скумбрии и красной икры</t>
+  </si>
+  <si>
+    <t>Рамен</t>
+  </si>
+  <si>
+    <t>Горячий рамен</t>
+  </si>
+  <si>
+    <t>Дайзу рамен</t>
+  </si>
+  <si>
+    <t>Рамен на курином бульоне с куриными подушками и яйцом аджитама, яично-пшеничной лапшой, ростки зелени, грибами муэр и зеленым луком</t>
+  </si>
+  <si>
+    <t>Унаги рамен</t>
+  </si>
+  <si>
+    <t>Рамен на нежном сливочном рыбном бульоне, с добавлением маринованного угря, грибов муэр, кунжута, зеленого лука</t>
+  </si>
+  <si>
+    <t>Чиизу Рамен</t>
+  </si>
+  <si>
+    <t>Рамен на насыщенном сырном бульоне на основе кокосового молока, с добавлением куриной грудинки, яично - пшеничной лапши, мисо-матадоре, ростков зелени, листьев вакамэ</t>
+  </si>
+  <si>
+    <t>Алкогольное меню</t>
+  </si>
+  <si>
+    <t>Алкогольные напитки</t>
+  </si>
+  <si>
+    <t>Красные вина</t>
+  </si>
+  <si>
+    <t>Для романтичного вечера</t>
+  </si>
+  <si>
+    <t>Шемен де Пап ля Ноблесс</t>
+  </si>
+  <si>
+    <t>Вино красное — фруктовое, среднетелое, выдержанное в дубе</t>
+  </si>
+  <si>
+    <t>Рипароссо Монтепульчано</t>
+  </si>
+  <si>
+    <t>Вино красное, сухое</t>
+  </si>
+  <si>
+    <t>Кьянти, Серристори</t>
+  </si>
+  <si>
+    <t>Вино красное — элегантное, комплексное, не выдержанное в дубе</t>
+  </si>
+  <si>
+    <t>Виски</t>
+  </si>
+  <si>
+    <t>Для интересных бесед</t>
+  </si>
+  <si>
+    <t>Джемисон</t>
+  </si>
+  <si>
+    <t>Классический купажированный виски, проходящий 4-хлетнюю выдержку в дубовых бочках</t>
+  </si>
+  <si>
+    <t>Джек Дэниелс</t>
+  </si>
+  <si>
+    <t>Характерен мягкий вкус, сочетает в себе карамельно-ванильные и древесные нотки. Легкий привкус дыма.</t>
+  </si>
+  <si>
+    <t>Чивас Ригал</t>
+  </si>
+  <si>
+    <t>Это купаж высококачественных солодовых и зерновых виски, выдержанных как минимум в течение 12 лет, что придает напитку роскошные нотки меда, ванили и спелых яблок.</t>
+  </si>
+  <si>
+    <t>Нарезка из ветчины, колбасных колечек, нескольких сортов сыра и фруктов</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2">
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
-      <color rgb="FF000000"/>
-      <sz val="10"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Montserrat"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -66,99 +188,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -359,425 +422,316 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col width="7.42578125" customWidth="1" min="1" max="1"/>
-    <col width="20.85546875" customWidth="1" min="2" max="2"/>
-    <col width="20.140625" customWidth="1" min="3" max="3"/>
-    <col width="21.7109375" customWidth="1" style="9" min="4" max="4"/>
-    <col width="77.7109375" customWidth="1" style="9" min="5" max="5"/>
-    <col width="12.5703125" customWidth="1" min="6" max="6"/>
+    <col min="1" max="1" width="7.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" style="9" customWidth="1"/>
+    <col min="5" max="5" width="77.7109375" style="9" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="5" t="inlineStr">
-        <is>
-          <t>96</t>
-        </is>
-      </c>
-      <c r="B1" s="5" t="inlineStr">
-        <is>
-          <t>Меню</t>
-        </is>
-      </c>
-      <c r="C1" s="5" t="inlineStr">
-        <is>
-          <t>Основное меню</t>
-        </is>
-      </c>
-      <c r="D1" s="8" t="n"/>
-      <c r="E1" s="8" t="n"/>
-      <c r="F1" s="5" t="n"/>
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A1" s="1">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="2"/>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="5" t="n"/>
-      <c r="B2" s="5" t="inlineStr">
-        <is>
-          <t>74</t>
-        </is>
-      </c>
-      <c r="C2" s="5" t="inlineStr">
-        <is>
-          <t>Холодные закуски</t>
-        </is>
-      </c>
-      <c r="D2" s="8" t="inlineStr">
-        <is>
-          <t>К пиву</t>
-        </is>
-      </c>
-      <c r="E2" s="8" t="n"/>
-      <c r="F2" s="5" t="n"/>
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A2" s="2"/>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="8"/>
+      <c r="F2" s="2"/>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="5" t="n"/>
-      <c r="B3" s="5" t="n"/>
-      <c r="C3" s="3" t="inlineStr">
-        <is>
-          <t>164</t>
-        </is>
-      </c>
-      <c r="D3" s="8" t="inlineStr">
-        <is>
-          <t>Сельдь Бисмарк</t>
-        </is>
-      </c>
-      <c r="E3" s="7" t="inlineStr">
-        <is>
-          <t>Традиционное немецкое блюдо из маринованной сельди</t>
-        </is>
-      </c>
-      <c r="F3" s="5" t="n">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A3" s="2"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="4">
         <v>182.99</v>
       </c>
     </row>
-    <row r="4" ht="16.5" customHeight="1">
-      <c r="A4" s="5" t="n"/>
-      <c r="B4" s="5" t="n"/>
-      <c r="C4" s="3" t="inlineStr">
-        <is>
-          <t>165</t>
-        </is>
-      </c>
-      <c r="D4" s="8" t="inlineStr">
-        <is>
-          <t>Мясная тарелка</t>
-        </is>
-      </c>
-      <c r="E4" s="6" t="inlineStr">
-        <is>
-          <t>Нарезка из ветчины, колбасных колечек, нескольких сортов сыра и фруктов</t>
-        </is>
-      </c>
-      <c r="F4" s="5" t="n">
+    <row r="4" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A4" s="2"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="3">
+        <v>2</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="4">
         <v>215.36</v>
       </c>
     </row>
-    <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="5" t="n"/>
-      <c r="B5" s="5" t="n"/>
-      <c r="C5" s="3" t="inlineStr">
-        <is>
-          <t>166</t>
-        </is>
-      </c>
-      <c r="D5" s="8" t="inlineStr">
-        <is>
-          <t>Рыбная тарелка</t>
-        </is>
-      </c>
-      <c r="E5" s="7" t="inlineStr">
-        <is>
-          <t>Нарезка из креветок, кальмаров, раковых шеек, гребешков, лосося, скумбрии и красной икры</t>
-        </is>
-      </c>
-      <c r="F5" s="5" t="n">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A5" s="2"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="3">
+        <v>3</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="4">
         <v>265.57</v>
       </c>
     </row>
-    <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="5" t="n"/>
-      <c r="B6" s="5" t="inlineStr">
-        <is>
-          <t>75</t>
-        </is>
-      </c>
-      <c r="C6" s="5" t="inlineStr">
-        <is>
-          <t>Рамен</t>
-        </is>
-      </c>
-      <c r="D6" s="8" t="inlineStr">
-        <is>
-          <t>Горячий рамен</t>
-        </is>
-      </c>
-      <c r="E6" s="7" t="n"/>
-      <c r="F6" s="5" t="n"/>
+    <row r="6" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A6" s="2"/>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="2"/>
     </row>
-    <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="5" t="n"/>
-      <c r="B7" s="5" t="n"/>
-      <c r="C7" s="5" t="inlineStr">
-        <is>
-          <t>167</t>
-        </is>
-      </c>
-      <c r="D7" s="8" t="inlineStr">
-        <is>
-          <t>Дайзу рамен</t>
-        </is>
-      </c>
-      <c r="E7" s="7" t="inlineStr">
-        <is>
-          <t>Рамен на курином бульоне с куриными подушками и яйцом аджитама, яично-пшеничной лапшой, ростки зелени, грибами муэр и зеленым луком</t>
-        </is>
-      </c>
-      <c r="F7" s="5" t="n">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="1">
         <v>166.47</v>
       </c>
     </row>
-    <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="5" t="n"/>
-      <c r="B8" s="5" t="n"/>
-      <c r="C8" s="5" t="inlineStr">
-        <is>
-          <t>168</t>
-        </is>
-      </c>
-      <c r="D8" s="8" t="inlineStr">
-        <is>
-          <t>Унаги рамен</t>
-        </is>
-      </c>
-      <c r="E8" s="7" t="inlineStr">
-        <is>
-          <t>Рамен на нежном сливочном рыбном бульоне, с добавлением маринованного угря, грибов муэр, кунжута, зеленого лука</t>
-        </is>
-      </c>
-      <c r="F8" s="5" t="n">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="1">
+        <v>2</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="1">
         <v>168.25</v>
       </c>
     </row>
-    <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="5" t="n"/>
-      <c r="B9" s="5" t="n"/>
-      <c r="C9" s="5" t="inlineStr">
-        <is>
-          <t>169</t>
-        </is>
-      </c>
-      <c r="D9" s="8" t="inlineStr">
-        <is>
-          <t>Чиизу Рамен</t>
-        </is>
-      </c>
-      <c r="E9" s="7" t="inlineStr">
-        <is>
-          <t>Рамен на насыщенном сырном бульоне на основе кокосового молока, с добавлением куриной грудинки, яично - пшеничной лапши, мисо-матадоре, ростков зелени, листьев вакамэ</t>
-        </is>
-      </c>
-      <c r="F9" s="5" t="n">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="1">
+        <v>3</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="1">
         <v>132.88</v>
       </c>
     </row>
-    <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="5" t="inlineStr">
-        <is>
-          <t>97</t>
-        </is>
-      </c>
-      <c r="B10" s="5" t="inlineStr">
-        <is>
-          <t>Алкогольное меню</t>
-        </is>
-      </c>
-      <c r="C10" s="5" t="inlineStr">
-        <is>
-          <t>Алкогольные напитки</t>
-        </is>
-      </c>
-      <c r="D10" s="8" t="n"/>
-      <c r="E10" s="7" t="n"/>
-      <c r="F10" s="5" t="n"/>
+    <row r="10" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A10" s="5">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="2"/>
     </row>
-    <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="5" t="n"/>
-      <c r="B11" s="5" t="inlineStr">
-        <is>
-          <t>76</t>
-        </is>
-      </c>
-      <c r="C11" s="5" t="inlineStr">
-        <is>
-          <t>Красные вина</t>
-        </is>
-      </c>
-      <c r="D11" s="8" t="inlineStr">
-        <is>
-          <t>Для романтичного вечера</t>
-        </is>
-      </c>
-      <c r="E11" s="7" t="n"/>
-      <c r="F11" s="5" t="n"/>
+    <row r="11" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A11" s="2"/>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="2"/>
     </row>
-    <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="5" t="n"/>
-      <c r="B12" s="5" t="n"/>
-      <c r="C12" s="3" t="inlineStr">
-        <is>
-          <t>170</t>
-        </is>
-      </c>
-      <c r="D12" s="8" t="inlineStr">
-        <is>
-          <t>Шемен де Пап ля Ноблесс</t>
-        </is>
-      </c>
-      <c r="E12" s="7" t="inlineStr">
-        <is>
-          <t>Вино красное — фруктовое, среднетелое, выдержанное в дубе</t>
-        </is>
-      </c>
-      <c r="F12" s="5" t="n">
+    <row r="12" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A12" s="2"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="3">
+        <v>1</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="1">
         <v>2700.79</v>
       </c>
     </row>
-    <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="5" t="n"/>
-      <c r="B13" s="5" t="n"/>
-      <c r="C13" s="3" t="inlineStr">
-        <is>
-          <t>171</t>
-        </is>
-      </c>
-      <c r="D13" s="8" t="inlineStr">
-        <is>
-          <t>Рипароссо Монтепульчано</t>
-        </is>
-      </c>
-      <c r="E13" s="7" t="inlineStr">
-        <is>
-          <t>Вино красное, сухое</t>
-        </is>
-      </c>
-      <c r="F13" s="5" t="n">
+    <row r="13" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A13" s="2"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="3">
+        <v>2</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="1">
         <v>3100.33</v>
       </c>
     </row>
-    <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="5" t="n"/>
-      <c r="B14" s="5" t="n"/>
-      <c r="C14" s="3" t="inlineStr">
-        <is>
-          <t>172</t>
-        </is>
-      </c>
-      <c r="D14" s="8" t="inlineStr">
-        <is>
-          <t>Кьянти, Серристори</t>
-        </is>
-      </c>
-      <c r="E14" s="7" t="inlineStr">
-        <is>
-          <t>Вино красное — элегантное, комплексное, не выдержанное в дубе</t>
-        </is>
-      </c>
-      <c r="F14" s="5" t="n">
+    <row r="14" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A14" s="2"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="3">
+        <v>3</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="1">
         <v>1850.42</v>
       </c>
     </row>
-    <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="5" t="n"/>
-      <c r="B15" s="5" t="inlineStr">
-        <is>
-          <t>77</t>
-        </is>
-      </c>
-      <c r="C15" s="5" t="inlineStr">
-        <is>
-          <t>Виски</t>
-        </is>
-      </c>
-      <c r="D15" s="8" t="inlineStr">
-        <is>
-          <t>Для интересных бесед</t>
-        </is>
-      </c>
-      <c r="E15" s="7" t="n"/>
-      <c r="F15" s="5" t="n"/>
+    <row r="15" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A15" s="2"/>
+      <c r="B15" s="1">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="7"/>
+      <c r="F15" s="2"/>
     </row>
-    <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="5" t="n"/>
-      <c r="B16" s="5" t="n"/>
-      <c r="C16" s="5" t="inlineStr">
-        <is>
-          <t>173</t>
-        </is>
-      </c>
-      <c r="D16" s="8" t="inlineStr">
-        <is>
-          <t>Джемисон</t>
-        </is>
-      </c>
-      <c r="E16" s="7" t="inlineStr">
-        <is>
-          <t>Классический купажированный виски, проходящий 4-хлетнюю выдержку в дубовых бочках</t>
-        </is>
-      </c>
-      <c r="F16" s="5" t="n">
+    <row r="16" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="1">
+        <v>1</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="1">
         <v>420.78</v>
       </c>
     </row>
-    <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="5" t="n"/>
-      <c r="B17" s="5" t="n"/>
-      <c r="C17" s="5" t="inlineStr">
-        <is>
-          <t>174</t>
-        </is>
-      </c>
-      <c r="D17" s="8" t="inlineStr">
-        <is>
-          <t>Джек Дэниелс</t>
-        </is>
-      </c>
-      <c r="E17" s="7" t="inlineStr">
-        <is>
-          <t>Характерен мягкий вкус, сочетает в себе карамельно-ванильные и древесные нотки. Легкий привкус дыма.</t>
-        </is>
-      </c>
-      <c r="F17" s="5" t="n">
+    <row r="17" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="1">
+        <v>2</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="1">
         <v>440.11</v>
       </c>
     </row>
-    <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="5" t="n"/>
-      <c r="B18" s="5" t="n"/>
-      <c r="C18" s="5" t="inlineStr">
-        <is>
-          <t>175</t>
-        </is>
-      </c>
-      <c r="D18" s="8" t="inlineStr">
-        <is>
-          <t>Чивас Ригал</t>
-        </is>
-      </c>
-      <c r="E18" s="7" t="inlineStr">
-        <is>
-          <t>Это купаж высококачественных солодовых и зерновых виски, выдержанных как минимум в течение 12 лет, что придает напитку роскошные нотки меда, ванили и спелых яблок.</t>
-        </is>
-      </c>
-      <c r="F18" s="5" t="n">
-        <v>520.08</v>
+    <row r="18" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="1">
+        <v>3</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="1">
+        <v>520.08000000000004</v>
       </c>
     </row>
-    <row r="19" ht="15.75" customHeight="1"/>
-    <row r="20" ht="15.75" customHeight="1"/>
-    <row r="21" ht="15.75" customHeight="1"/>
-    <row r="22" ht="15.75" customHeight="1"/>
-    <row r="23" ht="15.75" customHeight="1"/>
-    <row r="24" ht="15.75" customHeight="1"/>
-    <row r="25" ht="15.75" customHeight="1"/>
-    <row r="26" ht="15.75" customHeight="1"/>
-    <row r="27" ht="15.75" customHeight="1"/>
-    <row r="28" ht="15.75" customHeight="1"/>
-    <row r="29" ht="15.75" customHeight="1"/>
-    <row r="30" ht="15.75" customHeight="1"/>
-    <row r="31" ht="15.75" customHeight="1"/>
-    <row r="32" ht="15.75" customHeight="1"/>
+    <row r="19" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="20" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="21" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="22" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="23" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="24" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="25" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="26" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="27" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="28" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="29" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="30" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="31" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="32" spans="1:6" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Added test for details endpoint, added type hints for tasks
</commit_message>
<xml_diff>
--- a/admin/Menu.xlsx
+++ b/admin/Menu.xlsx
@@ -1,160 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Александр\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mjvwozj06heQVGmxYVZutM7iYW8Dw=="/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
-  <si>
-    <t>Меню</t>
-  </si>
-  <si>
-    <t>Основное меню</t>
-  </si>
-  <si>
-    <t>Холодные закуски</t>
-  </si>
-  <si>
-    <t>К пиву</t>
-  </si>
-  <si>
-    <t>Сельдь Бисмарк</t>
-  </si>
-  <si>
-    <t>Традиционное немецкое блюдо из маринованной сельди</t>
-  </si>
-  <si>
-    <t>Мясная тарелка</t>
-  </si>
-  <si>
-    <t>Рыбная тарелка</t>
-  </si>
-  <si>
-    <t>Нарезка из креветок, кальмаров, раковых шеек, гребешков, лосося, скумбрии и красной икры</t>
-  </si>
-  <si>
-    <t>Рамен</t>
-  </si>
-  <si>
-    <t>Горячий рамен</t>
-  </si>
-  <si>
-    <t>Дайзу рамен</t>
-  </si>
-  <si>
-    <t>Рамен на курином бульоне с куриными подушками и яйцом аджитама, яично-пшеничной лапшой, ростки зелени, грибами муэр и зеленым луком</t>
-  </si>
-  <si>
-    <t>Унаги рамен</t>
-  </si>
-  <si>
-    <t>Рамен на нежном сливочном рыбном бульоне, с добавлением маринованного угря, грибов муэр, кунжута, зеленого лука</t>
-  </si>
-  <si>
-    <t>Чиизу Рамен</t>
-  </si>
-  <si>
-    <t>Рамен на насыщенном сырном бульоне на основе кокосового молока, с добавлением куриной грудинки, яично - пшеничной лапши, мисо-матадоре, ростков зелени, листьев вакамэ</t>
-  </si>
-  <si>
-    <t>Алкогольное меню</t>
-  </si>
-  <si>
-    <t>Алкогольные напитки</t>
-  </si>
-  <si>
-    <t>Красные вина</t>
-  </si>
-  <si>
-    <t>Для романтичного вечера</t>
-  </si>
-  <si>
-    <t>Шемен де Пап ля Ноблесс</t>
-  </si>
-  <si>
-    <t>Вино красное — фруктовое, среднетелое, выдержанное в дубе</t>
-  </si>
-  <si>
-    <t>Рипароссо Монтепульчано</t>
-  </si>
-  <si>
-    <t>Вино красное, сухое</t>
-  </si>
-  <si>
-    <t>Кьянти, Серристори</t>
-  </si>
-  <si>
-    <t>Вино красное — элегантное, комплексное, не выдержанное в дубе</t>
-  </si>
-  <si>
-    <t>Виски</t>
-  </si>
-  <si>
-    <t>Для интересных бесед</t>
-  </si>
-  <si>
-    <t>Джемисон</t>
-  </si>
-  <si>
-    <t>Классический купажированный виски, проходящий 4-хлетнюю выдержку в дубовых бочках</t>
-  </si>
-  <si>
-    <t>Джек Дэниелс</t>
-  </si>
-  <si>
-    <t>Характерен мягкий вкус, сочетает в себе карамельно-ванильные и древесные нотки. Легкий привкус дыма.</t>
-  </si>
-  <si>
-    <t>Чивас Ригал</t>
-  </si>
-  <si>
-    <t>Это купаж высококачественных солодовых и зерновых виски, выдержанных как минимум в течение 12 лет, что придает напитку роскошные нотки меда, ванили и спелых яблок.</t>
-  </si>
-  <si>
-    <t>Нарезка из ветчины, колбасных колечек, нескольких сортов сыра и фруктов</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
+      <name val="Arial"/>
+      <color rgb="FF000000"/>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <name val="Montserrat"/>
+      <b val="1"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Montserrat"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -188,40 +66,99 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -422,316 +359,425 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1000"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" style="9" customWidth="1"/>
-    <col min="5" max="5" width="77.7109375" style="9" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col width="7.42578125" customWidth="1" min="1" max="1"/>
+    <col width="20.85546875" customWidth="1" min="2" max="2"/>
+    <col width="20.140625" customWidth="1" min="3" max="3"/>
+    <col width="21.7109375" customWidth="1" style="9" min="4" max="4"/>
+    <col width="77.7109375" customWidth="1" style="9" min="5" max="5"/>
+    <col width="12.5703125" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A1" s="1">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="2"/>
+    <row r="1" ht="15.75" customHeight="1">
+      <c r="A1" s="5" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="B1" s="5" t="inlineStr">
+        <is>
+          <t>Меню</t>
+        </is>
+      </c>
+      <c r="C1" s="5" t="inlineStr">
+        <is>
+          <t>Основное меню</t>
+        </is>
+      </c>
+      <c r="D1" s="8" t="n"/>
+      <c r="E1" s="8" t="n"/>
+      <c r="F1" s="5" t="n"/>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A2" s="2"/>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="2"/>
+    <row r="2" ht="15.75" customHeight="1">
+      <c r="A2" s="5" t="n"/>
+      <c r="B2" s="5" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="C2" s="5" t="inlineStr">
+        <is>
+          <t>Холодные закуски</t>
+        </is>
+      </c>
+      <c r="D2" s="8" t="inlineStr">
+        <is>
+          <t>К пиву</t>
+        </is>
+      </c>
+      <c r="E2" s="8" t="n"/>
+      <c r="F2" s="5" t="n"/>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A3" s="2"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="3">
-        <v>1</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="4">
+    <row r="3" ht="15.75" customHeight="1">
+      <c r="A3" s="5" t="n"/>
+      <c r="B3" s="5" t="n"/>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="D3" s="8" t="inlineStr">
+        <is>
+          <t>Сельдь Бисмарк</t>
+        </is>
+      </c>
+      <c r="E3" s="7" t="inlineStr">
+        <is>
+          <t>Традиционное немецкое блюдо из маринованной сельди</t>
+        </is>
+      </c>
+      <c r="F3" s="5" t="n">
         <v>182.99</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16.5" customHeight="1">
-      <c r="A4" s="2"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="3">
-        <v>2</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" s="4">
+    <row r="4" ht="16.5" customHeight="1">
+      <c r="A4" s="5" t="n"/>
+      <c r="B4" s="5" t="n"/>
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
+      </c>
+      <c r="D4" s="8" t="inlineStr">
+        <is>
+          <t>Мясная тарелка</t>
+        </is>
+      </c>
+      <c r="E4" s="6" t="inlineStr">
+        <is>
+          <t>Нарезка из ветчины, колбасных колечек, нескольких сортов сыра и фруктов</t>
+        </is>
+      </c>
+      <c r="F4" s="5" t="n">
         <v>215.36</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A5" s="2"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="3">
-        <v>3</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="4">
+    <row r="5" ht="15.75" customHeight="1">
+      <c r="A5" s="5" t="n"/>
+      <c r="B5" s="5" t="n"/>
+      <c r="C5" s="3" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="D5" s="8" t="inlineStr">
+        <is>
+          <t>Рыбная тарелка</t>
+        </is>
+      </c>
+      <c r="E5" s="7" t="inlineStr">
+        <is>
+          <t>Нарезка из креветок, кальмаров, раковых шеек, гребешков, лосося, скумбрии и красной икры</t>
+        </is>
+      </c>
+      <c r="F5" s="5" t="n">
         <v>265.57</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A6" s="2"/>
-      <c r="B6" s="1">
-        <v>2</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="2"/>
+    <row r="6" ht="15.75" customHeight="1">
+      <c r="A6" s="5" t="n"/>
+      <c r="B6" s="5" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="C6" s="5" t="inlineStr">
+        <is>
+          <t>Рамен</t>
+        </is>
+      </c>
+      <c r="D6" s="8" t="inlineStr">
+        <is>
+          <t>Горячий рамен</t>
+        </is>
+      </c>
+      <c r="E6" s="7" t="n"/>
+      <c r="F6" s="5" t="n"/>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="1">
-        <v>1</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="1">
+    <row r="7" ht="15.75" customHeight="1">
+      <c r="A7" s="5" t="n"/>
+      <c r="B7" s="5" t="n"/>
+      <c r="C7" s="5" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="D7" s="8" t="inlineStr">
+        <is>
+          <t>Дайзу рамен</t>
+        </is>
+      </c>
+      <c r="E7" s="7" t="inlineStr">
+        <is>
+          <t>Рамен на курином бульоне с куриными подушками и яйцом аджитама, яично-пшеничной лапшой, ростки зелени, грибами муэр и зеленым луком</t>
+        </is>
+      </c>
+      <c r="F7" s="5" t="n">
         <v>166.47</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="1">
-        <v>2</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="1">
+    <row r="8" ht="15.75" customHeight="1">
+      <c r="A8" s="5" t="n"/>
+      <c r="B8" s="5" t="n"/>
+      <c r="C8" s="5" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+      <c r="D8" s="8" t="inlineStr">
+        <is>
+          <t>Унаги рамен</t>
+        </is>
+      </c>
+      <c r="E8" s="7" t="inlineStr">
+        <is>
+          <t>Рамен на нежном сливочном рыбном бульоне, с добавлением маринованного угря, грибов муэр, кунжута, зеленого лука</t>
+        </is>
+      </c>
+      <c r="F8" s="5" t="n">
         <v>168.25</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="1">
-        <v>3</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="1">
+    <row r="9" ht="15.75" customHeight="1">
+      <c r="A9" s="5" t="n"/>
+      <c r="B9" s="5" t="n"/>
+      <c r="C9" s="5" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
+      <c r="D9" s="8" t="inlineStr">
+        <is>
+          <t>Чиизу Рамен</t>
+        </is>
+      </c>
+      <c r="E9" s="7" t="inlineStr">
+        <is>
+          <t>Рамен на насыщенном сырном бульоне на основе кокосового молока, с добавлением куриной грудинки, яично - пшеничной лапши, мисо-матадоре, ростков зелени, листьев вакамэ</t>
+        </is>
+      </c>
+      <c r="F9" s="5" t="n">
         <v>132.88</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A10" s="5">
-        <v>2</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="2"/>
+    <row r="10" ht="15.75" customHeight="1">
+      <c r="A10" s="5" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="B10" s="5" t="inlineStr">
+        <is>
+          <t>Алкогольное меню</t>
+        </is>
+      </c>
+      <c r="C10" s="5" t="inlineStr">
+        <is>
+          <t>Алкогольные напитки</t>
+        </is>
+      </c>
+      <c r="D10" s="8" t="n"/>
+      <c r="E10" s="7" t="n"/>
+      <c r="F10" s="5" t="n"/>
     </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A11" s="2"/>
-      <c r="B11" s="1">
-        <v>1</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="2"/>
+    <row r="11" ht="15.75" customHeight="1">
+      <c r="A11" s="5" t="n"/>
+      <c r="B11" s="5" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="C11" s="5" t="inlineStr">
+        <is>
+          <t>Красные вина</t>
+        </is>
+      </c>
+      <c r="D11" s="8" t="inlineStr">
+        <is>
+          <t>Для романтичного вечера</t>
+        </is>
+      </c>
+      <c r="E11" s="7" t="n"/>
+      <c r="F11" s="5" t="n"/>
     </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A12" s="2"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="3">
-        <v>1</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="1">
+    <row r="12" ht="15.75" customHeight="1">
+      <c r="A12" s="5" t="n"/>
+      <c r="B12" s="5" t="n"/>
+      <c r="C12" s="3" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="D12" s="8" t="inlineStr">
+        <is>
+          <t>Шемен де Пап ля Ноблесс</t>
+        </is>
+      </c>
+      <c r="E12" s="7" t="inlineStr">
+        <is>
+          <t>Вино красное — фруктовое, среднетелое, выдержанное в дубе</t>
+        </is>
+      </c>
+      <c r="F12" s="5" t="n">
         <v>2700.79</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A13" s="2"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="3">
-        <v>2</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" s="1">
+    <row r="13" ht="15.75" customHeight="1">
+      <c r="A13" s="5" t="n"/>
+      <c r="B13" s="5" t="n"/>
+      <c r="C13" s="3" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
+      <c r="D13" s="8" t="inlineStr">
+        <is>
+          <t>Рипароссо Монтепульчано</t>
+        </is>
+      </c>
+      <c r="E13" s="7" t="inlineStr">
+        <is>
+          <t>Вино красное, сухое</t>
+        </is>
+      </c>
+      <c r="F13" s="5" t="n">
         <v>3100.33</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A14" s="2"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="3">
-        <v>3</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F14" s="1">
+    <row r="14" ht="15.75" customHeight="1">
+      <c r="A14" s="5" t="n"/>
+      <c r="B14" s="5" t="n"/>
+      <c r="C14" s="3" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="D14" s="8" t="inlineStr">
+        <is>
+          <t>Кьянти, Серристори</t>
+        </is>
+      </c>
+      <c r="E14" s="7" t="inlineStr">
+        <is>
+          <t>Вино красное — элегантное, комплексное, не выдержанное в дубе</t>
+        </is>
+      </c>
+      <c r="F14" s="5" t="n">
         <v>1850.42</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A15" s="2"/>
-      <c r="B15" s="1">
-        <v>2</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="7"/>
-      <c r="F15" s="2"/>
+    <row r="15" ht="15.75" customHeight="1">
+      <c r="A15" s="5" t="n"/>
+      <c r="B15" s="5" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="C15" s="5" t="inlineStr">
+        <is>
+          <t>Виски</t>
+        </is>
+      </c>
+      <c r="D15" s="8" t="inlineStr">
+        <is>
+          <t>Для интересных бесед</t>
+        </is>
+      </c>
+      <c r="E15" s="7" t="n"/>
+      <c r="F15" s="5" t="n"/>
     </row>
-    <row r="16" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="1">
-        <v>1</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F16" s="1">
+    <row r="16" ht="15.75" customHeight="1">
+      <c r="A16" s="5" t="n"/>
+      <c r="B16" s="5" t="n"/>
+      <c r="C16" s="5" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
+      </c>
+      <c r="D16" s="8" t="inlineStr">
+        <is>
+          <t>Джемисон</t>
+        </is>
+      </c>
+      <c r="E16" s="7" t="inlineStr">
+        <is>
+          <t>Классический купажированный виски, проходящий 4-хлетнюю выдержку в дубовых бочках</t>
+        </is>
+      </c>
+      <c r="F16" s="5" t="n">
         <v>420.78</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="1">
-        <v>2</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F17" s="1">
+    <row r="17" ht="15.75" customHeight="1">
+      <c r="A17" s="5" t="n"/>
+      <c r="B17" s="5" t="n"/>
+      <c r="C17" s="5" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="D17" s="8" t="inlineStr">
+        <is>
+          <t>Джек Дэниелс</t>
+        </is>
+      </c>
+      <c r="E17" s="7" t="inlineStr">
+        <is>
+          <t>Характерен мягкий вкус, сочетает в себе карамельно-ванильные и древесные нотки. Легкий привкус дыма.</t>
+        </is>
+      </c>
+      <c r="F17" s="5" t="n">
         <v>440.11</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="1">
-        <v>3</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" s="1">
-        <v>520.08000000000004</v>
+    <row r="18" ht="15.75" customHeight="1">
+      <c r="A18" s="5" t="n"/>
+      <c r="B18" s="5" t="n"/>
+      <c r="C18" s="5" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
+      </c>
+      <c r="D18" s="8" t="inlineStr">
+        <is>
+          <t>Чивас Ригал</t>
+        </is>
+      </c>
+      <c r="E18" s="7" t="inlineStr">
+        <is>
+          <t>Это купаж высококачественных солодовых и зерновых виски, выдержанных как минимум в течение 12 лет, что придает напитку роскошные нотки меда, ванили и спелых яблок.</t>
+        </is>
+      </c>
+      <c r="F18" s="5" t="n">
+        <v>520.08</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="22" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="23" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="25" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="26" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="27" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="28" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="30" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="31" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="32" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="19" ht="15.75" customHeight="1"/>
+    <row r="20" ht="15.75" customHeight="1"/>
+    <row r="21" ht="15.75" customHeight="1"/>
+    <row r="22" ht="15.75" customHeight="1"/>
+    <row r="23" ht="15.75" customHeight="1"/>
+    <row r="24" ht="15.75" customHeight="1"/>
+    <row r="25" ht="15.75" customHeight="1"/>
+    <row r="26" ht="15.75" customHeight="1"/>
+    <row r="27" ht="15.75" customHeight="1"/>
+    <row r="28" ht="15.75" customHeight="1"/>
+    <row r="29" ht="15.75" customHeight="1"/>
+    <row r="30" ht="15.75" customHeight="1"/>
+    <row r="31" ht="15.75" customHeight="1"/>
+    <row r="32" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>

</xml_diff>